<commit_message>
Preserve uncertainty info when regionalizing datasets. Distinguish between preserving ecoinvent and imports uncertainty.
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-battery-capacity.xlsx
+++ b/premise/data/additional_inventories/lci-battery-capacity.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/Github/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6CBD25A-E903-2945-8CE6-B8E5BCF92E02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68FF2860-B80F-ED45-BBD1-C9D83E9F3527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Battery - NMC" sheetId="1" r:id="rId1"/>
@@ -758,8 +758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N266"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A150" workbookViewId="0">
-      <selection activeCell="D176" sqref="D176"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4879,8 +4879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E327F433-64CA-4C75-A0BC-FFEEC2922B0D}">
   <dimension ref="A1:N204"/>
   <sheetViews>
-    <sheetView topLeftCell="A120" workbookViewId="0">
-      <selection activeCell="A165" sqref="A165"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="J106" sqref="J106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6229,12 +6229,12 @@
         <v>51.546391752577321</v>
       </c>
       <c r="I90" s="3">
-        <f>1/(0.02)</f>
-        <v>50</v>
-      </c>
-      <c r="J90" s="3">
         <f>1/(0.06)</f>
         <v>16.666666666666668</v>
+      </c>
+      <c r="J90" s="3">
+        <f>1/(0.019)</f>
+        <v>52.631578947368425</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.2">
@@ -6265,12 +6265,12 @@
         <v>-51.546391752577321</v>
       </c>
       <c r="I91" s="3">
-        <f>-1/(0.06)</f>
+        <f>-1*J90</f>
+        <v>-52.631578947368425</v>
+      </c>
+      <c r="J91" s="3">
+        <f>-1*I90</f>
         <v>-16.666666666666668</v>
-      </c>
-      <c r="J91" s="3">
-        <f>-1/(0.02)</f>
-        <v>-50</v>
       </c>
       <c r="K91" t="b">
         <v>1</v>
@@ -6436,12 +6436,12 @@
         <v>33.333333333333336</v>
       </c>
       <c r="I104" s="3">
+        <f>1/(0.032)</f>
+        <v>31.25</v>
+      </c>
+      <c r="J104" s="3">
         <f>1/(0.027)</f>
         <v>37.037037037037038</v>
-      </c>
-      <c r="J104" s="3">
-        <f>1/(0.032)</f>
-        <v>31.25</v>
       </c>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.2">
@@ -6472,12 +6472,12 @@
         <v>-33.333333333333336</v>
       </c>
       <c r="I105" s="3">
-        <f>-J104</f>
+        <f>-1*J104</f>
+        <v>-37.037037037037038</v>
+      </c>
+      <c r="J105" s="3">
+        <f>-1*I104</f>
         <v>-31.25</v>
-      </c>
-      <c r="J105" s="3">
-        <f>-I104</f>
-        <v>-37.037037037037038</v>
       </c>
       <c r="K105" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Fix uncertainty params for a few datasets. Created datasets to provide 1 kWh of electricity from stationary batteries. Renamed product of battery markets to "electricity storage capacity".
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-battery-capacity.xlsx
+++ b/premise/data/additional_inventories/lci-battery-capacity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/Github/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68FF2860-B80F-ED45-BBD1-C9D83E9F3527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E883C0AF-51F8-5E43-ABF0-9A5C7FFB13D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Battery - NMC'!$A$1:$N$266</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Battery - stationary'!$A$1:$N$204</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Battery - stationary'!$A$1:$N$203</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1344" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1371" uniqueCount="115">
   <si>
     <t>Activity</t>
   </si>
@@ -373,6 +373,18 @@
   </si>
   <si>
     <t>market group for electricity, low voltage</t>
+  </si>
+  <si>
+    <t>electricity storage capacity</t>
+  </si>
+  <si>
+    <t>electricity supply, from stationary battery (CONT scenario)</t>
+  </si>
+  <si>
+    <t>This dataset provides a market average for 1 kWh of battery gross capacity (NOT net). It is based on shares provided by Schlichenmaier &amp; Naegler (2022) https://doi.org/10.1016/j.egyr.2022.11.025.</t>
+  </si>
+  <si>
+    <t>This dataset provides a kilowatt hour from a stationary battery system. Assumed lifetime : 2'500 cycles, or 2'500 kWh. Min: 1'500 cycles. Max: 5'000 cycles. Includes charging and discharging losses of 33%.</t>
   </si>
 </sst>
 </file>
@@ -758,8 +770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N266"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView topLeftCell="A235" workbookViewId="0">
+      <selection activeCell="F253" sqref="F253:F266"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -813,7 +825,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
@@ -895,7 +907,7 @@
       </c>
       <c r="F12" t="str">
         <f>B7</f>
-        <v>electricity, low voltage</v>
+        <v>electricity storage capacity</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
@@ -1012,7 +1024,7 @@
         <v>5</v>
       </c>
       <c r="B20" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
@@ -1093,7 +1105,7 @@
       </c>
       <c r="F25" t="str">
         <f>B20</f>
-        <v>electricity, low voltage</v>
+        <v>electricity storage capacity</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
@@ -1210,7 +1222,7 @@
         <v>5</v>
       </c>
       <c r="B33" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
@@ -1291,7 +1303,7 @@
       </c>
       <c r="F38" t="str">
         <f>B33</f>
-        <v>electricity, low voltage</v>
+        <v>electricity storage capacity</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
@@ -1408,7 +1420,7 @@
         <v>5</v>
       </c>
       <c r="B46" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E46" s="3"/>
     </row>
@@ -1491,7 +1503,7 @@
       </c>
       <c r="F51" t="str">
         <f>B46</f>
-        <v>electricity, low voltage</v>
+        <v>electricity storage capacity</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.2">
@@ -1608,7 +1620,7 @@
         <v>5</v>
       </c>
       <c r="B59" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.2">
@@ -1689,7 +1701,7 @@
       </c>
       <c r="F64" t="str">
         <f>B59</f>
-        <v>electricity, low voltage</v>
+        <v>electricity storage capacity</v>
       </c>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.2">
@@ -1806,7 +1818,7 @@
         <v>5</v>
       </c>
       <c r="B72" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.2">
@@ -1887,7 +1899,7 @@
       </c>
       <c r="F77" t="str">
         <f>B72</f>
-        <v>electricity, low voltage</v>
+        <v>electricity storage capacity</v>
       </c>
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.2">
@@ -2004,7 +2016,7 @@
         <v>5</v>
       </c>
       <c r="B85" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.2">
@@ -2085,7 +2097,7 @@
       </c>
       <c r="F90" t="str">
         <f>B85</f>
-        <v>electricity, low voltage</v>
+        <v>electricity storage capacity</v>
       </c>
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.2">
@@ -2202,7 +2214,7 @@
         <v>5</v>
       </c>
       <c r="B98" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E98" s="3"/>
     </row>
@@ -2283,7 +2295,7 @@
       </c>
       <c r="F103" t="str">
         <f>B98</f>
-        <v>electricity, low voltage</v>
+        <v>electricity storage capacity</v>
       </c>
     </row>
     <row r="104" spans="1:14" x14ac:dyDescent="0.2">
@@ -2400,7 +2412,7 @@
         <v>5</v>
       </c>
       <c r="B111" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="112" spans="1:14" x14ac:dyDescent="0.2">
@@ -2481,7 +2493,7 @@
       </c>
       <c r="F116" t="str">
         <f>B111</f>
-        <v>electricity, low voltage</v>
+        <v>electricity storage capacity</v>
       </c>
     </row>
     <row r="117" spans="1:14" x14ac:dyDescent="0.2">
@@ -2598,7 +2610,7 @@
         <v>5</v>
       </c>
       <c r="B124" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="125" spans="1:14" x14ac:dyDescent="0.2">
@@ -2679,7 +2691,7 @@
       </c>
       <c r="F129" t="str">
         <f>B124</f>
-        <v>electricity, low voltage</v>
+        <v>electricity storage capacity</v>
       </c>
     </row>
     <row r="130" spans="1:14" x14ac:dyDescent="0.2">
@@ -2796,7 +2808,7 @@
         <v>5</v>
       </c>
       <c r="B137" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="138" spans="1:14" x14ac:dyDescent="0.2">
@@ -2876,7 +2888,7 @@
       </c>
       <c r="F142" t="str">
         <f>B137</f>
-        <v>electricity, low voltage</v>
+        <v>electricity storage capacity</v>
       </c>
     </row>
     <row r="143" spans="1:14" x14ac:dyDescent="0.2">
@@ -2993,7 +3005,7 @@
         <v>5</v>
       </c>
       <c r="B150" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E150" s="3"/>
     </row>
@@ -3074,7 +3086,7 @@
       </c>
       <c r="F155" t="str">
         <f>B150</f>
-        <v>electricity, low voltage</v>
+        <v>electricity storage capacity</v>
       </c>
     </row>
     <row r="156" spans="1:14" x14ac:dyDescent="0.2">
@@ -3191,7 +3203,7 @@
         <v>5</v>
       </c>
       <c r="B163" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="164" spans="1:14" x14ac:dyDescent="0.2">
@@ -3276,7 +3288,7 @@
       </c>
       <c r="F168" t="str">
         <f>B163</f>
-        <v>electricity, low voltage</v>
+        <v>electricity storage capacity</v>
       </c>
     </row>
     <row r="169" spans="1:14" x14ac:dyDescent="0.2">
@@ -3393,7 +3405,7 @@
         <v>5</v>
       </c>
       <c r="B176" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="177" spans="1:11" x14ac:dyDescent="0.2">
@@ -3466,7 +3478,7 @@
         <v>13</v>
       </c>
       <c r="F181" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="G181" s="1"/>
       <c r="H181" s="1"/>
@@ -3491,7 +3503,7 @@
         <v>14</v>
       </c>
       <c r="F182" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="183" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -3511,7 +3523,7 @@
         <v>14</v>
       </c>
       <c r="F183" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="184" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -3531,7 +3543,7 @@
         <v>14</v>
       </c>
       <c r="F184" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="185" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -3551,7 +3563,7 @@
         <v>14</v>
       </c>
       <c r="F185" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="186" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -3571,7 +3583,7 @@
         <v>14</v>
       </c>
       <c r="F186" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="187" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -3591,7 +3603,7 @@
         <v>14</v>
       </c>
       <c r="F187" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="188" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -3611,7 +3623,7 @@
         <v>14</v>
       </c>
       <c r="F188" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="189" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -3631,7 +3643,7 @@
         <v>14</v>
       </c>
       <c r="F189" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="190" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -3651,7 +3663,7 @@
         <v>14</v>
       </c>
       <c r="F190" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="191" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -3671,7 +3683,7 @@
         <v>14</v>
       </c>
       <c r="F191" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="192" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -3691,7 +3703,7 @@
         <v>14</v>
       </c>
       <c r="F192" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="193" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -3711,7 +3723,7 @@
         <v>14</v>
       </c>
       <c r="F193" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="194" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -3731,7 +3743,7 @@
         <v>14</v>
       </c>
       <c r="F194" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="196" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -3771,7 +3783,7 @@
         <v>5</v>
       </c>
       <c r="B200" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="201" spans="1:11" x14ac:dyDescent="0.2">
@@ -3844,7 +3856,7 @@
         <v>13</v>
       </c>
       <c r="F205" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="G205" s="1"/>
       <c r="H205" s="1"/>
@@ -3869,7 +3881,7 @@
         <v>14</v>
       </c>
       <c r="F206" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="207" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -3889,7 +3901,7 @@
         <v>14</v>
       </c>
       <c r="F207" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="208" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -3909,7 +3921,7 @@
         <v>14</v>
       </c>
       <c r="F208" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="209" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -3929,7 +3941,7 @@
         <v>14</v>
       </c>
       <c r="F209" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="210" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -3949,7 +3961,7 @@
         <v>14</v>
       </c>
       <c r="F210" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="211" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -3969,7 +3981,7 @@
         <v>14</v>
       </c>
       <c r="F211" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="212" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -3989,7 +4001,7 @@
         <v>14</v>
       </c>
       <c r="F212" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="213" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -4009,7 +4021,7 @@
         <v>14</v>
       </c>
       <c r="F213" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="214" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -4029,7 +4041,7 @@
         <v>14</v>
       </c>
       <c r="F214" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="215" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -4049,7 +4061,7 @@
         <v>14</v>
       </c>
       <c r="F215" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="216" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -4069,7 +4081,7 @@
         <v>14</v>
       </c>
       <c r="F216" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="217" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -4089,7 +4101,7 @@
         <v>14</v>
       </c>
       <c r="F217" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="218" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -4109,7 +4121,7 @@
         <v>14</v>
       </c>
       <c r="F218" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="220" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -4149,7 +4161,7 @@
         <v>5</v>
       </c>
       <c r="B224" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="225" spans="1:11" x14ac:dyDescent="0.2">
@@ -4222,7 +4234,7 @@
         <v>13</v>
       </c>
       <c r="F229" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="G229" s="1"/>
       <c r="H229" s="1"/>
@@ -4247,7 +4259,7 @@
         <v>14</v>
       </c>
       <c r="F230" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="231" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -4267,7 +4279,7 @@
         <v>14</v>
       </c>
       <c r="F231" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="232" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -4287,7 +4299,7 @@
         <v>14</v>
       </c>
       <c r="F232" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="233" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -4307,7 +4319,7 @@
         <v>14</v>
       </c>
       <c r="F233" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="234" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -4327,7 +4339,7 @@
         <v>14</v>
       </c>
       <c r="F234" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="235" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -4347,7 +4359,7 @@
         <v>14</v>
       </c>
       <c r="F235" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="236" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -4367,7 +4379,7 @@
         <v>14</v>
       </c>
       <c r="F236" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="237" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -4387,7 +4399,7 @@
         <v>14</v>
       </c>
       <c r="F237" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="238" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -4407,7 +4419,7 @@
         <v>14</v>
       </c>
       <c r="F238" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="239" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -4427,7 +4439,7 @@
         <v>14</v>
       </c>
       <c r="F239" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="240" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -4447,7 +4459,7 @@
         <v>14</v>
       </c>
       <c r="F240" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="241" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -4467,7 +4479,7 @@
         <v>14</v>
       </c>
       <c r="F241" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="242" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -4487,7 +4499,7 @@
         <v>14</v>
       </c>
       <c r="F242" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="244" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -4527,7 +4539,7 @@
         <v>5</v>
       </c>
       <c r="B248" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="249" spans="1:11" x14ac:dyDescent="0.2">
@@ -4600,7 +4612,7 @@
         <v>13</v>
       </c>
       <c r="F253" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="G253" s="1"/>
       <c r="H253" s="1"/>
@@ -4625,7 +4637,7 @@
         <v>14</v>
       </c>
       <c r="F254" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="255" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -4645,7 +4657,7 @@
         <v>14</v>
       </c>
       <c r="F255" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="256" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -4665,7 +4677,7 @@
         <v>14</v>
       </c>
       <c r="F256" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="257" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -4685,7 +4697,7 @@
         <v>14</v>
       </c>
       <c r="F257" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="258" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -4705,7 +4717,7 @@
         <v>14</v>
       </c>
       <c r="F258" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="259" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -4725,7 +4737,7 @@
         <v>14</v>
       </c>
       <c r="F259" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="260" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -4745,7 +4757,7 @@
         <v>14</v>
       </c>
       <c r="F260" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="261" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -4765,7 +4777,7 @@
         <v>14</v>
       </c>
       <c r="F261" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="262" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -4785,7 +4797,7 @@
         <v>14</v>
       </c>
       <c r="F262" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="263" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -4805,7 +4817,7 @@
         <v>14</v>
       </c>
       <c r="F263" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="264" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -4825,7 +4837,7 @@
         <v>14</v>
       </c>
       <c r="F264" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="265" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -4845,7 +4857,7 @@
         <v>14</v>
       </c>
       <c r="F265" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="266" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -4865,7 +4877,7 @@
         <v>14</v>
       </c>
       <c r="F266" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -4877,10 +4889,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E327F433-64CA-4C75-A0BC-FFEEC2922B0D}">
-  <dimension ref="A1:N204"/>
+  <dimension ref="A1:N203"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="J106" sqref="J106"/>
+    <sheetView tabSelected="1" topLeftCell="A164" workbookViewId="0">
+      <selection activeCell="J189" sqref="J189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4927,7 +4939,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -5009,7 +5021,7 @@
       </c>
       <c r="F10" t="str">
         <f>B5</f>
-        <v>electricity, low voltage</v>
+        <v>electricity storage capacity</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
@@ -5126,7 +5138,7 @@
         <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
@@ -5207,7 +5219,7 @@
       </c>
       <c r="F23" t="str">
         <f>B18</f>
-        <v>electricity, low voltage</v>
+        <v>electricity storage capacity</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
@@ -5324,7 +5336,7 @@
         <v>5</v>
       </c>
       <c r="B31" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
@@ -5405,7 +5417,7 @@
       </c>
       <c r="F36" t="str">
         <f>B31</f>
-        <v>electricity, low voltage</v>
+        <v>electricity storage capacity</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
@@ -5522,7 +5534,7 @@
         <v>5</v>
       </c>
       <c r="B44" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E44" s="3"/>
     </row>
@@ -5605,7 +5617,7 @@
       </c>
       <c r="F49" t="str">
         <f>B44</f>
-        <v>electricity, low voltage</v>
+        <v>electricity storage capacity</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.2">
@@ -5722,7 +5734,7 @@
         <v>5</v>
       </c>
       <c r="B57" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.2">
@@ -5803,7 +5815,7 @@
       </c>
       <c r="F62" t="str">
         <f>B57</f>
-        <v>electricity, low voltage</v>
+        <v>electricity storage capacity</v>
       </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.2">
@@ -5920,7 +5932,7 @@
         <v>5</v>
       </c>
       <c r="B70" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.2">
@@ -6001,7 +6013,7 @@
       </c>
       <c r="F75" t="str">
         <f>B70</f>
-        <v>electricity, low voltage</v>
+        <v>electricity storage capacity</v>
       </c>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.2">
@@ -6118,7 +6130,7 @@
         <v>5</v>
       </c>
       <c r="B84" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E84" s="3"/>
     </row>
@@ -6198,7 +6210,7 @@
       </c>
       <c r="F89" t="str">
         <f>B84</f>
-        <v>electricity, low voltage</v>
+        <v>electricity storage capacity</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.2">
@@ -6325,7 +6337,7 @@
         <v>5</v>
       </c>
       <c r="B98" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E98" s="3"/>
     </row>
@@ -6405,7 +6417,7 @@
       </c>
       <c r="F103" t="str">
         <f>B98</f>
-        <v>electricity, low voltage</v>
+        <v>electricity storage capacity</v>
       </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.2">
@@ -6526,7 +6538,7 @@
         <v>5</v>
       </c>
       <c r="B112" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E112" s="3"/>
     </row>
@@ -6607,7 +6619,7 @@
       </c>
       <c r="F117" t="str">
         <f>B112</f>
-        <v>electricity, low voltage</v>
+        <v>electricity storage capacity</v>
       </c>
     </row>
     <row r="118" spans="1:14" x14ac:dyDescent="0.2">
@@ -6724,7 +6736,7 @@
         <v>5</v>
       </c>
       <c r="B125" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="126" spans="1:14" x14ac:dyDescent="0.2">
@@ -6809,7 +6821,7 @@
       </c>
       <c r="F130" t="str">
         <f>B125</f>
-        <v>electricity, low voltage</v>
+        <v>electricity storage capacity</v>
       </c>
     </row>
     <row r="131" spans="1:11" x14ac:dyDescent="0.2">
@@ -6930,7 +6942,7 @@
         <v>5</v>
       </c>
       <c r="B139" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="140" spans="1:11" x14ac:dyDescent="0.2">
@@ -7013,7 +7025,7 @@
       </c>
       <c r="F144" t="str">
         <f>B139</f>
-        <v>electricity, low voltage</v>
+        <v>electricity storage capacity</v>
       </c>
       <c r="G144" s="1"/>
       <c r="H144" s="1"/>
@@ -7038,7 +7050,7 @@
         <v>14</v>
       </c>
       <c r="F145" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="146" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -7058,7 +7070,7 @@
         <v>14</v>
       </c>
       <c r="F146" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="147" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -7078,7 +7090,7 @@
         <v>14</v>
       </c>
       <c r="F147" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="148" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -7098,7 +7110,7 @@
         <v>14</v>
       </c>
       <c r="F148" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="149" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -7118,7 +7130,7 @@
         <v>14</v>
       </c>
       <c r="F149" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="150" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -7138,7 +7150,7 @@
         <v>14</v>
       </c>
       <c r="F150" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="151" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -7158,7 +7170,7 @@
         <v>14</v>
       </c>
       <c r="F151" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="152" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -7178,7 +7190,7 @@
         <v>14</v>
       </c>
       <c r="F152" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="153" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -7198,7 +7210,7 @@
         <v>14</v>
       </c>
       <c r="F153" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="G153" s="6"/>
       <c r="H153" s="6"/>
@@ -7223,114 +7235,121 @@
         <v>14</v>
       </c>
       <c r="F154" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="155" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A155" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="B155">
-        <v>0.33</v>
-      </c>
-      <c r="C155" t="s">
-        <v>15</v>
-      </c>
-      <c r="D155" t="s">
-        <v>3</v>
-      </c>
-      <c r="E155" t="s">
-        <v>14</v>
-      </c>
-      <c r="F155" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="157" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A157" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B157" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="156" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A156" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B156" s="2" t="s">
         <v>102</v>
+      </c>
+    </row>
+    <row r="157" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>1</v>
+      </c>
+      <c r="B157" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="158" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B158" t="s">
-        <v>108</v>
+        <v>3</v>
       </c>
     </row>
     <row r="159" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>2</v>
-      </c>
-      <c r="B159" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="B159">
+        <v>1</v>
       </c>
     </row>
     <row r="160" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>4</v>
-      </c>
-      <c r="B160">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="B160" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="161" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B161" t="s">
-        <v>109</v>
+        <v>15</v>
       </c>
     </row>
     <row r="162" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B162" t="s">
-        <v>15</v>
+        <v>107</v>
       </c>
     </row>
     <row r="163" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A163" t="s">
-        <v>8</v>
-      </c>
-      <c r="B163" t="s">
-        <v>107</v>
-      </c>
+      <c r="A163" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B163" s="1"/>
+      <c r="C163" s="1"/>
+      <c r="D163" s="1"/>
+      <c r="E163" s="1"/>
+      <c r="F163" s="1"/>
+      <c r="G163" s="1"/>
     </row>
     <row r="164" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B164" s="1"/>
-      <c r="C164" s="1"/>
-      <c r="D164" s="1"/>
-      <c r="E164" s="1"/>
-      <c r="F164" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D164" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E164" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F164" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="G164" s="1"/>
+      <c r="H164" s="1"/>
+      <c r="I164" s="1"/>
+      <c r="J164" s="1"/>
+      <c r="K164" s="1"/>
     </row>
     <row r="165" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A165" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B165" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C165" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D165" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E165" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F165" s="1" t="s">
-        <v>5</v>
+      <c r="A165" t="str">
+        <f>B156</f>
+        <v>market for battery capacity, stationary (TC scenario)</v>
+      </c>
+      <c r="B165">
+        <v>1</v>
+      </c>
+      <c r="C165" t="s">
+        <v>15</v>
+      </c>
+      <c r="D165" t="s">
+        <v>3</v>
+      </c>
+      <c r="E165" t="s">
+        <v>13</v>
+      </c>
+      <c r="F165" t="str">
+        <f>B160</f>
+        <v>electricity storage capacity</v>
       </c>
       <c r="G165" s="1"/>
       <c r="H165" s="1"/>
@@ -7338,13 +7357,12 @@
       <c r="J165" s="1"/>
       <c r="K165" s="1"/>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A166" t="str">
-        <f>B157</f>
-        <v>market for battery capacity, stationary (TC scenario)</v>
+    <row r="166" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A166" s="6" t="s">
+        <v>83</v>
       </c>
       <c r="B166">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C166" t="s">
         <v>15</v>
@@ -7353,21 +7371,15 @@
         <v>3</v>
       </c>
       <c r="E166" t="s">
-        <v>13</v>
-      </c>
-      <c r="F166" t="str">
-        <f>B161</f>
-        <v>electricity, low voltage</v>
-      </c>
-      <c r="G166" s="1"/>
-      <c r="H166" s="1"/>
-      <c r="I166" s="1"/>
-      <c r="J166" s="1"/>
-      <c r="K166" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="F166" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="167" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A167" s="6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B167">
         <v>0</v>
@@ -7382,12 +7394,12 @@
         <v>14</v>
       </c>
       <c r="F167" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="168" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A168" s="6" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B168">
         <v>0</v>
@@ -7402,12 +7414,12 @@
         <v>14</v>
       </c>
       <c r="F168" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="169" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A169" s="6" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B169">
         <v>0</v>
@@ -7422,12 +7434,12 @@
         <v>14</v>
       </c>
       <c r="F169" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="170" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A170" s="6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B170">
         <v>0</v>
@@ -7442,12 +7454,12 @@
         <v>14</v>
       </c>
       <c r="F170" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="171" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A171" s="6" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B171">
         <v>0</v>
@@ -7462,12 +7474,12 @@
         <v>14</v>
       </c>
       <c r="F171" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="172" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A172" s="6" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B172">
         <v>0</v>
@@ -7482,12 +7494,12 @@
         <v>14</v>
       </c>
       <c r="F172" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="173" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A173" s="6" t="s">
-        <v>89</v>
+        <v>106</v>
       </c>
       <c r="B173">
         <v>0</v>
@@ -7502,14 +7514,14 @@
         <v>14</v>
       </c>
       <c r="F173" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="174" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A174" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="B174">
+        <v>94</v>
+      </c>
+      <c r="B174" s="6">
         <v>0</v>
       </c>
       <c r="C174" t="s">
@@ -7522,14 +7534,16 @@
         <v>14</v>
       </c>
       <c r="F174" t="s">
-        <v>109</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="G174" s="6"/>
+      <c r="H174" s="6"/>
     </row>
     <row r="175" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A175" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="B175" s="6">
+        <v>100</v>
+      </c>
+      <c r="B175">
         <v>0</v>
       </c>
       <c r="C175" t="s">
@@ -7542,63 +7556,217 @@
         <v>14</v>
       </c>
       <c r="F175" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="176" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A176" s="4"/>
+    </row>
+    <row r="177" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A177" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B177" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="178" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
+        <v>1</v>
+      </c>
+      <c r="B178" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="179" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
+        <v>2</v>
+      </c>
+      <c r="B179" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="180" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A180" t="s">
+        <v>4</v>
+      </c>
+      <c r="B180">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A181" t="s">
+        <v>5</v>
+      </c>
+      <c r="B181" t="s">
         <v>109</v>
       </c>
-      <c r="G175" s="6"/>
-      <c r="H175" s="6"/>
-    </row>
-    <row r="176" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A176" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="B176">
-        <v>0</v>
-      </c>
-      <c r="C176" t="s">
-        <v>15</v>
-      </c>
-      <c r="D176" t="s">
-        <v>3</v>
-      </c>
-      <c r="E176" t="s">
-        <v>14</v>
-      </c>
-      <c r="F176" t="s">
+    </row>
+    <row r="182" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A182" t="s">
+        <v>6</v>
+      </c>
+      <c r="B182" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="183" spans="1:11" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A183" t="s">
+        <v>8</v>
+      </c>
+      <c r="B183" t="s">
+        <v>107</v>
+      </c>
+      <c r="C183"/>
+      <c r="D183"/>
+      <c r="E183"/>
+      <c r="F183"/>
+      <c r="G183"/>
+      <c r="H183"/>
+      <c r="I183"/>
+      <c r="J183"/>
+      <c r="K183"/>
+    </row>
+    <row r="184" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A184" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B184" s="1"/>
+      <c r="C184" s="1"/>
+      <c r="D184" s="1"/>
+      <c r="E184" s="1"/>
+      <c r="F184" s="1"/>
+      <c r="G184" s="1"/>
+    </row>
+    <row r="185" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A185" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C185" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D185" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E185" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F185" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G185" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H185" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I185" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="J185" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K185" s="1"/>
+    </row>
+    <row r="186" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A186" t="str">
+        <f>B177</f>
+        <v>electricity supply, from stationary battery (CONT scenario)</v>
+      </c>
+      <c r="B186">
+        <v>1</v>
+      </c>
+      <c r="C186" t="s">
+        <v>15</v>
+      </c>
+      <c r="D186" t="s">
+        <v>3</v>
+      </c>
+      <c r="E186" t="s">
+        <v>13</v>
+      </c>
+      <c r="F186" t="str">
+        <f>B181</f>
+        <v>electricity, low voltage</v>
+      </c>
+      <c r="G186">
+        <v>0</v>
+      </c>
+      <c r="I186" s="1"/>
+      <c r="J186" s="1"/>
+      <c r="K186" s="1"/>
+    </row>
+    <row r="187" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A187" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B187">
+        <f>1/2500</f>
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="C187" t="s">
+        <v>15</v>
+      </c>
+      <c r="D187" t="s">
+        <v>3</v>
+      </c>
+      <c r="E187" t="s">
+        <v>14</v>
+      </c>
+      <c r="F187" t="s">
+        <v>111</v>
+      </c>
+      <c r="G187">
+        <v>5</v>
+      </c>
+      <c r="H187">
+        <f>B187</f>
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="I187">
+        <f>1/5000</f>
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="J187">
+        <f>1/1500</f>
+        <v>6.6666666666666664E-4</v>
+      </c>
+    </row>
+    <row r="188" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A188" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B188">
+        <v>0.33</v>
+      </c>
+      <c r="C188" t="s">
+        <v>15</v>
+      </c>
+      <c r="D188" t="s">
+        <v>3</v>
+      </c>
+      <c r="E188" t="s">
+        <v>14</v>
+      </c>
+      <c r="F188" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="177" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A177" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="B177">
+      <c r="G188">
+        <v>5</v>
+      </c>
+      <c r="H188">
+        <f>B188</f>
         <v>0.33</v>
       </c>
-      <c r="C177" t="s">
-        <v>15</v>
-      </c>
-      <c r="D177" t="s">
-        <v>3</v>
-      </c>
-      <c r="E177" t="s">
-        <v>14</v>
-      </c>
-      <c r="F177" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="178" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A178" s="4"/>
-    </row>
-    <row r="179" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A179" s="4"/>
-    </row>
-    <row r="180" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A180" s="5"/>
-    </row>
-    <row r="182" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A182" s="2"/>
-      <c r="B182" s="2"/>
+      <c r="I188">
+        <v>0.25</v>
+      </c>
+      <c r="J188">
+        <v>0.4</v>
+      </c>
     </row>
     <row r="189" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A189" s="1"/>
@@ -7608,26 +7776,20 @@
       <c r="E189" s="1"/>
       <c r="F189" s="1"/>
       <c r="G189" s="1"/>
+      <c r="H189" s="1"/>
+      <c r="I189" s="1"/>
+      <c r="J189" s="1"/>
+      <c r="K189" s="1"/>
     </row>
     <row r="190" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A190" s="1"/>
-      <c r="B190" s="1"/>
-      <c r="C190" s="1"/>
-      <c r="D190" s="1"/>
-      <c r="E190" s="1"/>
-      <c r="F190" s="1"/>
       <c r="G190" s="1"/>
       <c r="H190" s="1"/>
       <c r="I190" s="1"/>
       <c r="J190" s="1"/>
       <c r="K190" s="1"/>
     </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="G191" s="1"/>
-      <c r="H191" s="1"/>
-      <c r="I191" s="1"/>
-      <c r="J191" s="1"/>
-      <c r="K191" s="1"/>
+    <row r="191" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A191" s="6"/>
     </row>
     <row r="192" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A192" s="6"/>
@@ -7652,26 +7814,23 @@
     </row>
     <row r="199" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A199" s="6"/>
+      <c r="B199" s="6"/>
+      <c r="G199" s="6"/>
     </row>
     <row r="200" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A200" s="6"/>
-      <c r="B200" s="6"/>
-      <c r="G200" s="6"/>
     </row>
     <row r="201" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A201" s="6"/>
+      <c r="A201" s="4"/>
     </row>
     <row r="202" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A202" s="4"/>
     </row>
     <row r="203" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A203" s="4"/>
-    </row>
-    <row r="204" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A204" s="5"/>
+      <c r="A203" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N204" xr:uid="{E327F433-64CA-4C75-A0BC-FFEEC2922B0D}"/>
+  <autoFilter ref="A1:N203" xr:uid="{E327F433-64CA-4C75-A0BC-FFEEC2922B0D}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix uncertainty values in battery datasets.
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-battery-capacity.xlsx
+++ b/premise/data/additional_inventories/lci-battery-capacity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/Github/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E883C0AF-51F8-5E43-ABF0-9A5C7FFB13D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4290815-5539-434A-B68F-C88551189D42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -770,8 +770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N266"/>
   <sheetViews>
-    <sheetView topLeftCell="A235" workbookViewId="0">
-      <selection activeCell="F253" sqref="F253:F266"/>
+    <sheetView topLeftCell="A125" workbookViewId="0">
+      <selection activeCell="J157" sqref="J157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2722,12 +2722,12 @@
         <v>8.8888888888888893</v>
       </c>
       <c r="I130" s="3">
-        <f>1/(0.5*75%)</f>
-        <v>2.6666666666666665</v>
+        <f>1/(0.18*75%)</f>
+        <v>7.4074074074074066</v>
       </c>
       <c r="J130" s="3">
-        <f>1/(0.14*75%)</f>
-        <v>9.5238095238095237</v>
+        <f>1/(0.12*75%)</f>
+        <v>11.111111111111111</v>
       </c>
     </row>
     <row r="131" spans="1:14" x14ac:dyDescent="0.2">
@@ -2758,12 +2758,12 @@
         <v>-8.8888888888888893</v>
       </c>
       <c r="I131" s="3">
-        <f>-1/(0.14*75%)</f>
-        <v>-9.5238095238095237</v>
+        <f>-1/(0.12*75%)</f>
+        <v>-11.111111111111111</v>
       </c>
       <c r="J131" s="3">
-        <f>-1/(0.5*75%)</f>
-        <v>-2.6666666666666665</v>
+        <f>-1/(0.18*75%)</f>
+        <v>-7.4074074074074066</v>
       </c>
       <c r="K131" t="b">
         <v>1</v>
@@ -3117,12 +3117,12 @@
         <v>8.3333333333333339</v>
       </c>
       <c r="I156" s="3">
-        <f>1/(0.22*75%)</f>
-        <v>6.0606060606060606</v>
+        <f>1/(0.18*75%)</f>
+        <v>7.4074074074074066</v>
       </c>
       <c r="J156" s="3">
-        <f>1/(0.16*75%)</f>
-        <v>8.3333333333333339</v>
+        <f>1/(0.12*75%)</f>
+        <v>11.111111111111111</v>
       </c>
     </row>
     <row r="157" spans="1:14" x14ac:dyDescent="0.2">
@@ -3153,12 +3153,12 @@
         <v>-8.3333333333333339</v>
       </c>
       <c r="I157" s="3">
-        <f>-1/(0.16*75%)</f>
-        <v>-8.3333333333333339</v>
+        <f>-1/(0.12*75%)</f>
+        <v>-11.111111111111111</v>
       </c>
       <c r="J157" s="3">
-        <f>-1/(0.22*75%)</f>
-        <v>-6.0606060606060606</v>
+        <f>-1/(0.18*75%)</f>
+        <v>-7.4074074074074066</v>
       </c>
       <c r="K157" t="b">
         <v>1</v>
@@ -4891,8 +4891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E327F433-64CA-4C75-A0BC-FFEEC2922B0D}">
   <dimension ref="A1:N203"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A164" workbookViewId="0">
-      <selection activeCell="J189" sqref="J189"/>
+    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="J120" sqref="J120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6650,12 +6650,12 @@
         <v>8.3333333333333339</v>
       </c>
       <c r="I118" s="3">
-        <f>1/(0.22*75%)</f>
-        <v>6.0606060606060606</v>
+        <f>1/(0.18*75%)</f>
+        <v>7.4074074074074066</v>
       </c>
       <c r="J118" s="3">
-        <f>1/(0.16*75%)</f>
-        <v>8.3333333333333339</v>
+        <f>1/(0.12*75%)</f>
+        <v>11.111111111111111</v>
       </c>
     </row>
     <row r="119" spans="1:14" x14ac:dyDescent="0.2">
@@ -6686,12 +6686,12 @@
         <v>-8.3333333333333339</v>
       </c>
       <c r="I119" s="3">
-        <f>-1/(0.16*75%)</f>
-        <v>-8.3333333333333339</v>
+        <f>-1/(0.12*75%)</f>
+        <v>-11.111111111111111</v>
       </c>
       <c r="J119" s="3">
-        <f>-1/(0.22*75%)</f>
-        <v>-6.0606060606060606</v>
+        <f>-1/(0.18*75%)</f>
+        <v>-7.4074074074074066</v>
       </c>
       <c r="K119" t="b">
         <v>1</v>

</xml_diff>